<commit_message>
Thêm tạo tran cho ImportExcel
</commit_message>
<xml_diff>
--- a/src/main/resources/report_templates/PNK.xlsx
+++ b/src/main/resources/report_templates/PNK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\MeuPro\MeUVipPro\src\main\resources\report_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836046D1-8E30-4FC6-8F48-3E9EA92605F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6C1847-F76F-495B-BA5A-D06E2A477FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Mẫu số 02-VT</t>
   </si>
@@ -203,18 +203,6 @@
     <t>Thực xuất</t>
   </si>
   <si>
-    <t xml:space="preserve">${dataset.indexOf (e)+1} </t>
-  </si>
-  <si>
-    <t>${e.type+ e.model}</t>
-  </si>
-  <si>
-    <t>${e.productCode}</t>
-  </si>
-  <si>
-    <t>Cái</t>
-  </si>
-  <si>
     <t>${e.quantity}</t>
   </si>
   <si>
@@ -224,19 +212,28 @@
     <t>${total2}</t>
   </si>
   <si>
-    <t>${toUserName}</t>
+    <t>${dayString}</t>
   </si>
   <si>
-    <t>${address1}</t>
+    <t>${outDeptName}</t>
   </si>
   <si>
-    <t>${fromWarehouseName}</t>
+    <t>${outDeptAddress}</t>
   </si>
   <si>
-    <t>${address2}</t>
+    <t xml:space="preserve">${e.index} </t>
   </si>
   <si>
-    <t>${dayString}</t>
+    <t>${e.unit}</t>
+  </si>
+  <si>
+    <t>${e.name}</t>
+  </si>
+  <si>
+    <t>${e.code}</t>
+  </si>
+  <si>
+    <t>${e.realQuantity}</t>
   </si>
 </sst>
 </file>
@@ -787,34 +784,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -848,6 +817,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -857,7 +830,31 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1075,20 +1072,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" customWidth="1"/>
     <col min="4" max="6" width="4.44140625" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" customWidth="1"/>
-    <col min="9" max="11" width="10" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="0.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="10" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" customWidth="1"/>
     <col min="13" max="14" width="4.44140625" customWidth="1"/>
     <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
@@ -1103,11 +1101,11 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
@@ -1135,11 +1133,11 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -1167,11 +1165,11 @@
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" s="55" t="s">
+      <c r="J3" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1197,11 +1195,11 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="55" t="s">
+      <c r="J4" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -1246,20 +1244,20 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -1278,16 +1276,16 @@
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="53" t="s">
-        <v>42</v>
+      <c r="C7" s="72" t="s">
+        <v>34</v>
       </c>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
       <c r="K7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1343,7 +1341,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1375,7 +1373,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1439,7 +1437,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1471,7 +1469,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1516,42 +1514,42 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="58" t="s">
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="60" t="s">
+      <c r="J15" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="48" t="s">
+      <c r="K15" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="49"/>
+      <c r="L15" s="70"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="59"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="72"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="65"/>
       <c r="K16" s="26" t="s">
         <v>19</v>
       </c>
@@ -1563,41 +1561,41 @@
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="68"/>
-      <c r="I17" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="L17" s="28" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:26" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="31"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="71"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="63"/>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
       <c r="K18" s="33"/>
@@ -1635,10 +1633,10 @@
       <c r="I20" s="42"/>
       <c r="J20" s="43"/>
       <c r="K20" s="44" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L20" s="44" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -1865,11 +1863,11 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="J31" s="50" t="s">
+      <c r="J31" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -1886,24 +1884,24 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="52" t="s">
+      <c r="A32" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="52" t="s">
+      <c r="B32" s="60"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="H32" s="51"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="51"/>
-      <c r="K32" s="52" t="s">
+      <c r="H32" s="60"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="L32" s="51"/>
+      <c r="L32" s="60"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
@@ -1920,24 +1918,24 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="51"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="57" t="s">
+      <c r="B33" s="60"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="51"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="57" t="s">
+      <c r="H33" s="60"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="L33" s="51"/>
+      <c r="L33" s="60"/>
       <c r="M33" s="23"/>
       <c r="N33" s="23"/>
       <c r="O33" s="23"/>
@@ -1982,20 +1980,20 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="52"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="51"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="52" t="s">
+      <c r="A35" s="64"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="L35" s="51"/>
+      <c r="L35" s="60"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
@@ -29033,6 +29031,25 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="G33:H33"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:H16"/>
     <mergeCell ref="I15:I16"/>
@@ -29043,25 +29060,6 @@
     <mergeCell ref="C32:F32"/>
     <mergeCell ref="G32:H32"/>
     <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="C7:J7"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.20833333333333334" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>